<commit_message>
Add vox piece, remove impact director, update WID tech note and data
</commit_message>
<xml_diff>
--- a/data/AdvaniSummersTarrant_UKTopIncomes_WIDTechnicalNote_Data.xlsx
+++ b/data/AdvaniSummersTarrant_UKTopIncomes_WIDTechnicalNote_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sandbox\MeasuringTopIncomes\Drafts\WID technical note\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local_user\Documents\WorkHD\MeasuringTopIncomes\Drafts\WID technical note\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA5E020-925B-4989-B3CA-7953DBDD5950}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD80288-4A2A-431A-BDF7-3C151641A264}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{E551DC49-9B49-4831-9479-62EF28A1AA56}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{E551DC49-9B49-4831-9479-62EF28A1AA56}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="44">
   <si>
     <t xml:space="preserve">Population control </t>
   </si>
@@ -226,6 +226,9 @@
       </rPr>
       <t>CAGE Working Paper 490.</t>
     </r>
+  </si>
+  <si>
+    <t>Pre-tax top shares including realised capital gains (%)</t>
   </si>
 </sst>
 </file>
@@ -633,28 +636,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D16E31D-3752-4785-A482-63241B25E6C6}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.5" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -669,19 +672,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B050249-AC1A-4916-89CB-E5D85F721C0B}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -689,7 +694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -697,7 +702,7 @@
         <v>46802000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -705,7 +710,7 @@
         <v>46919000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -713,7 +718,7 @@
         <v>47071000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -721,7 +726,7 @@
         <v>47347000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -729,7 +734,7 @@
         <v>47652000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -737,7 +742,7 @@
         <v>48007000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -745,7 +750,7 @@
         <v>48306000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -753,7 +758,7 @@
         <v>48625000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -761,7 +766,7 @@
         <v>48980000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
@@ -769,7 +774,7 @@
         <v>49436000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -777,7 +782,7 @@
         <v>49850000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
@@ -785,7 +790,7 @@
         <v>50266000</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -793,7 +798,7 @@
         <v>50648000</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -801,7 +806,7 @@
         <v>50996000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
@@ -809,7 +814,7 @@
         <v>51781000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -817,7 +822,7 @@
         <v>52169000</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
@@ -825,7 +830,7 @@
         <v>52491000</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
@@ -833,7 +838,7 @@
         <v>52798000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
@@ -841,7 +846,7 @@
         <v>53189000</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
@@ -849,7 +854,7 @@
         <v>53579000</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
@@ -857,7 +862,7 @@
         <v>53971000</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
@@ -874,21 +879,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFAD970-F2A8-417F-BA00-3675A5F0FD66}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="29.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.6796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -902,7 +909,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -916,7 +923,7 @@
         <v>475775.41832882259</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -930,7 +937,7 @@
         <v>512360.14740859123</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -944,7 +951,7 @@
         <v>553485.24783381331</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -958,7 +965,7 @@
         <v>588475.37561024958</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -972,7 +979,7 @@
         <v>642701.88957921998</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -986,7 +993,7 @@
         <v>657324.1283558266</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1000,77 +1007,77 @@
         <v>679903.84584996663</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="7">
-        <v>665043.00881768379</v>
+        <v>665033.58865569381</v>
       </c>
       <c r="C10" s="7">
-        <v>521057.01517582388</v>
+        <v>521047.59501383384</v>
       </c>
       <c r="D10" s="7">
-        <v>680784.6048215779</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
+        <v>680775.18465958792</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="7">
-        <v>729676.73521579045</v>
+        <v>729672.15384509147</v>
       </c>
       <c r="C11" s="7">
-        <v>570425.17541876272</v>
+        <v>570420.59404806374</v>
       </c>
       <c r="D11" s="7">
-        <v>750581.02736095525</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
+        <v>750576.44599025627</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="7">
-        <v>796671.38244668429</v>
+        <v>796668.35196319094</v>
       </c>
       <c r="C12" s="7">
-        <v>619351.63912610849</v>
+        <v>619348.60864261515</v>
       </c>
       <c r="D12" s="7">
-        <v>824642.52017844282</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
+        <v>824639.48969494947</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="7">
-        <v>849293.0597314419</v>
+        <v>849287.20391328097</v>
       </c>
       <c r="C13" s="7">
-        <v>658671.89183428232</v>
+        <v>658666.03601612139</v>
       </c>
       <c r="D13" s="7">
-        <v>888508.13623853575</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.75">
+        <v>888502.28042037482</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="7">
-        <v>912832.12943556567</v>
+        <v>912828.67688211065</v>
       </c>
       <c r="C14" s="7">
-        <v>706538.43952790066</v>
+        <v>706534.98697444552</v>
       </c>
       <c r="D14" s="7">
-        <v>979449.30328140978</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.75">
+        <v>979445.85072795476</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -1078,7 +1085,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1092,7 +1099,7 @@
         <v>944970.65818269958</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
@@ -1106,21 +1113,21 @@
         <v>937790.57297153433</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="7">
-        <v>951379.77637976001</v>
+        <v>951249.36885674007</v>
       </c>
       <c r="C18" s="7">
-        <v>748241.92215769459</v>
+        <v>748113.13546705153</v>
       </c>
       <c r="D18" s="7">
-        <v>971674.11486475996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.75">
+        <v>971543.70734174002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
@@ -1134,7 +1141,7 @@
         <v>997078.64674919215</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
@@ -1148,7 +1155,7 @@
         <v>1055037.1927074227</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
@@ -1162,7 +1169,7 @@
         <v>1088818.1943148733</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
@@ -1176,32 +1183,32 @@
         <v>1161857.8462745005</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="7">
-        <v>1141120.4247505369</v>
+        <v>1141089.8431397646</v>
       </c>
       <c r="C23" s="7">
-        <v>913625.00406573317</v>
+        <v>913595.30168744014</v>
       </c>
       <c r="D23" s="7">
-        <v>1188979.8274715368</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.75">
+        <v>1188949.2458607645</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="7">
-        <v>1178067.1564204372</v>
+        <v>1178067.578536235</v>
       </c>
       <c r="C24" s="7">
-        <v>951724.14547876501</v>
+        <v>951723.70502621564</v>
       </c>
       <c r="D24" s="7">
-        <v>1232781.0068664372</v>
+        <v>1232781.428982235</v>
       </c>
     </row>
   </sheetData>
@@ -1213,16 +1220,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71C1347-5E75-4519-8281-C6C5016E9046}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1245,7 +1254,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1268,7 +1277,7 @@
         <v>2.9894690151757768</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1291,7 +1300,7 @@
         <v>3.085618269301027</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1314,7 +1323,7 @@
         <v>3.3631285289156549</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1337,7 +1346,7 @@
         <v>3.4466272731861993</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1360,7 +1369,7 @@
         <v>3.5336815884218589</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1383,7 +1392,7 @@
         <v>3.3408685437959078</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1406,122 +1415,122 @@
         <v>3.1353475808446585</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="6">
-        <v>41.105288775372365</v>
+        <v>41.105871029390073</v>
       </c>
       <c r="C10" s="6">
-        <v>28.71994922988133</v>
+        <v>28.720356046286852</v>
       </c>
       <c r="D10" s="6">
-        <v>13.143299512750305</v>
+        <v>13.143485686821215</v>
       </c>
       <c r="E10" s="6">
-        <v>9.5249935662154765</v>
+        <v>9.5251284871937223</v>
       </c>
       <c r="F10" s="6">
-        <v>4.5672898541022793</v>
+        <v>4.5673545494966392</v>
       </c>
       <c r="G10" s="6">
-        <v>3.2922072129691133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
+        <v>3.2922538468922409</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="6">
-        <v>40.610642321823939</v>
+        <v>40.610897302647615</v>
       </c>
       <c r="C11" s="6">
-        <v>28.400119367337957</v>
+        <v>28.400297682316857</v>
       </c>
       <c r="D11" s="6">
-        <v>13.219887720224758</v>
+        <v>13.219970723537857</v>
       </c>
       <c r="E11" s="6">
-        <v>9.6260285163658317</v>
+        <v>9.6260889550227819</v>
       </c>
       <c r="F11" s="6">
-        <v>4.6752995553078511</v>
+        <v>4.6753289099711459</v>
       </c>
       <c r="G11" s="6">
-        <v>3.4002115754502533</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
+        <v>3.4002329242568372</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="6">
-        <v>41.411176210399233</v>
+        <v>41.411333736282671</v>
       </c>
       <c r="C12" s="6">
-        <v>29.402105383363001</v>
+        <v>29.402217227387951</v>
       </c>
       <c r="D12" s="6">
-        <v>14.143589612007402</v>
+        <v>14.143643413460353</v>
       </c>
       <c r="E12" s="6">
-        <v>10.405003548615493</v>
+        <v>10.405043128688462</v>
       </c>
       <c r="F12" s="6">
-        <v>5.1469015659855462</v>
+        <v>5.1469211445218335</v>
       </c>
       <c r="G12" s="6">
-        <v>3.7632831099424009</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
+        <v>3.7632974252686182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="6">
-        <v>41.839508664321876</v>
+        <v>41.8397971468912</v>
       </c>
       <c r="C13" s="6">
-        <v>29.990063039797679</v>
+        <v>29.990269820678147</v>
       </c>
       <c r="D13" s="6">
-        <v>14.794043154198928</v>
+        <v>14.79414515882843</v>
       </c>
       <c r="E13" s="6">
-        <v>10.998239267927159</v>
+        <v>10.998315100565337</v>
       </c>
       <c r="F13" s="6">
-        <v>5.5632276243514225</v>
+        <v>5.5632659826938138</v>
       </c>
       <c r="G13" s="6">
-        <v>4.088443001492517</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
+        <v>4.0884711912246452</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="6">
-        <v>41.986715533891257</v>
+        <v>41.986874338476888</v>
       </c>
       <c r="C14" s="6">
-        <v>30.316612821783053</v>
+        <v>30.316727487030754</v>
       </c>
       <c r="D14" s="6">
-        <v>15.22323473863789</v>
+        <v>15.223292316837419</v>
       </c>
       <c r="E14" s="6">
-        <v>11.43409744333024</v>
+        <v>11.434140690035379</v>
       </c>
       <c r="F14" s="6">
-        <v>5.9666871041610179</v>
+        <v>5.9667096717103272</v>
       </c>
       <c r="G14" s="6">
-        <v>4.4486422699858803</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
+        <v>4.4486590958981553</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1532,7 +1541,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1555,7 +1564,7 @@
         <v>4.9806237841522183</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1578,30 +1587,30 @@
         <v>3.7505191133818787</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="6">
-        <v>40.955917325301726</v>
+        <v>40.961532004171708</v>
       </c>
       <c r="C18" s="6">
-        <v>28.898026149692278</v>
+        <v>28.901987802791588</v>
       </c>
       <c r="D18" s="6">
-        <v>13.552038078205351</v>
+        <v>13.553895937748297</v>
       </c>
       <c r="E18" s="6">
-        <v>9.949404619262701</v>
+        <v>9.9507685909555086</v>
       </c>
       <c r="F18" s="6">
-        <v>5.0329303547485695</v>
+        <v>5.0336203231234062</v>
       </c>
       <c r="G18" s="6">
-        <v>3.7375871608008557</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
+        <v>3.7380995495599638</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1624,7 +1633,7 @@
         <v>3.5482221300327761</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1647,7 +1656,7 @@
         <v>4.4236816132654591</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1670,7 +1679,7 @@
         <v>4.2020289855531354</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1693,30 +1702,30 @@
         <v>4.6634865580347729</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
-        <v>40.467607244095966</v>
+        <v>40.468691790261254</v>
       </c>
       <c r="C23" s="6">
-        <v>28.98870306351138</v>
+        <v>28.98947997099085</v>
       </c>
       <c r="D23" s="6">
-        <v>14.113600820463029</v>
+        <v>14.11397906994924</v>
       </c>
       <c r="E23" s="6">
-        <v>10.617640908514375</v>
+        <v>10.617925465040345</v>
       </c>
       <c r="F23" s="6">
-        <v>5.5944132658847989</v>
+        <v>5.5945631981359929</v>
       </c>
       <c r="G23" s="6">
-        <v>4.2100420342299545</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
+        <v>4.2101548648432487</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1748,16 +1757,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677A3F08-2064-478E-BD14-112C99177F39}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1780,7 +1791,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1803,7 +1814,7 @@
         <v>2.3921695530320535</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1826,7 +1837,7 @@
         <v>2.5787135352231561</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1849,7 +1860,7 @@
         <v>2.6993255170704655</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1872,7 +1883,7 @@
         <v>2.7327511426963289</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1895,7 +1906,7 @@
         <v>2.8045192321410797</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1918,7 +1929,7 @@
         <v>2.6912376702580234</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1941,122 +1952,122 @@
         <v>2.5336722475114741</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="6">
-        <v>37.05552552284697</v>
+        <v>37.05619545982853</v>
       </c>
       <c r="C10" s="6">
-        <v>25.074733996272293</v>
+        <v>25.075187329246791</v>
       </c>
       <c r="D10" s="6">
-        <v>10.90711297495559</v>
+        <v>10.907310167634437</v>
       </c>
       <c r="E10" s="6">
-        <v>7.8231263228191024</v>
+        <v>7.8232677592597168</v>
       </c>
       <c r="F10" s="6">
-        <v>3.7248473549141128</v>
+        <v>3.7249146974482827</v>
       </c>
       <c r="G10" s="6">
-        <v>2.6915555986755311</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
+        <v>2.6916042600454086</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="6">
-        <v>36.602412661715142</v>
+        <v>36.602706636411412</v>
       </c>
       <c r="C11" s="6">
-        <v>24.761708810930411</v>
+        <v>24.761907686231176</v>
       </c>
       <c r="D11" s="6">
-        <v>10.949554187544571</v>
+        <v>10.949642129612661</v>
       </c>
       <c r="E11" s="6">
-        <v>7.882963879290827</v>
+        <v>7.8830271918361916</v>
       </c>
       <c r="F11" s="6">
-        <v>3.7846221569560132</v>
+        <v>3.7846525533989848</v>
       </c>
       <c r="G11" s="6">
-        <v>2.7474908898727399</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
+        <v>2.7475129565273977</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="6">
-        <v>37.352925653435584</v>
+        <v>37.353108421949216</v>
       </c>
       <c r="C12" s="6">
-        <v>25.64979676302454</v>
+        <v>25.649922267925358</v>
       </c>
       <c r="D12" s="6">
-        <v>11.76350609320067</v>
+        <v>11.763563652240187</v>
       </c>
       <c r="E12" s="6">
-        <v>8.5675060017176854</v>
+        <v>8.5675479226732758</v>
       </c>
       <c r="F12" s="6">
-        <v>4.1963164902965708</v>
+        <v>4.1963370229460013</v>
       </c>
       <c r="G12" s="6">
-        <v>3.0657825928417362</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
+        <v>3.0657975937691817</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="6">
-        <v>37.817930836552229</v>
+        <v>37.818267053867366</v>
       </c>
       <c r="C13" s="6">
-        <v>26.242261260195097</v>
+        <v>26.242494564937818</v>
       </c>
       <c r="D13" s="6">
-        <v>12.406657986710009</v>
+        <v>12.406768287118989</v>
       </c>
       <c r="E13" s="6">
-        <v>9.1454267970180645</v>
+        <v>9.1455081037097692</v>
       </c>
       <c r="F13" s="6">
-        <v>4.5872768845962124</v>
+        <v>4.5873176674175831</v>
       </c>
       <c r="G13" s="6">
-        <v>3.3621807574134084</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
+        <v>3.3622106486148109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="6">
-        <v>37.871480056531823</v>
+        <v>37.871665119284167</v>
       </c>
       <c r="C14" s="6">
-        <v>26.446929480130166</v>
+        <v>26.447058715680335</v>
       </c>
       <c r="D14" s="6">
-        <v>12.731666577243725</v>
+        <v>12.731728791798194</v>
       </c>
       <c r="E14" s="6">
-        <v>9.4798041696220654</v>
+        <v>9.4798504936275894</v>
       </c>
       <c r="F14" s="6">
-        <v>4.9034185711519678</v>
+        <v>4.9034425321942976</v>
       </c>
       <c r="G14" s="6">
-        <v>3.6428025177684948</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
+        <v>3.6428203186851529</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2067,7 +2078,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2090,7 +2101,7 @@
         <v>4.0489230385635926</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -2113,30 +2124,30 @@
         <v>2.7029683170658991</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="6">
-        <v>36.020470498701449</v>
+        <v>36.026671375241378</v>
       </c>
       <c r="C18" s="6">
-        <v>24.247417761290194</v>
+        <v>24.251591922312198</v>
       </c>
       <c r="D18" s="6">
-        <v>10.369769423611089</v>
+        <v>10.371554565755352</v>
       </c>
       <c r="E18" s="6">
-        <v>7.4050030630809012</v>
+        <v>7.4062778246022321</v>
       </c>
       <c r="F18" s="6">
-        <v>3.6047716862249759</v>
+        <v>3.6053922429215284</v>
       </c>
       <c r="G18" s="6">
-        <v>2.6575912568164846</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
+        <v>2.6580487576500098</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2159,7 +2170,7 @@
         <v>2.495355268762371</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2182,7 +2193,7 @@
         <v>3.2528286222654206</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2205,7 +2216,7 @@
         <v>3.0964547390114787</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2228,50 +2239,50 @@
         <v>3.450870955067336</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
-        <v>35.270154487033039</v>
+        <v>35.271301173611981</v>
       </c>
       <c r="C23" s="6">
-        <v>24.001958285537437</v>
+        <v>24.002738625851638</v>
       </c>
       <c r="D23" s="6">
-        <v>10.71433810890964</v>
+        <v>10.714686448402064</v>
       </c>
       <c r="E23" s="6">
-        <v>7.9102991008761077</v>
+        <v>7.9105562767786886</v>
       </c>
       <c r="F23" s="6">
-        <v>4.1134902772054147</v>
+        <v>4.1136240130555146</v>
       </c>
       <c r="G23" s="6">
-        <v>3.1048792994770387</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
+        <v>3.104980243844131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="6">
-        <v>35.175177611296981</v>
+        <v>35.175148455512847</v>
       </c>
       <c r="C24" s="6">
-        <v>24.01094639255297</v>
+        <v>24.010956597880977</v>
       </c>
       <c r="D24" s="6">
-        <v>10.928024659749283</v>
+        <v>10.928029616428191</v>
       </c>
       <c r="E24" s="6">
-        <v>8.1105189098581398</v>
+        <v>8.1105226199284584</v>
       </c>
       <c r="F24" s="6">
-        <v>4.2733624977973657</v>
+        <v>4.2733644653872629</v>
       </c>
       <c r="G24" s="6">
-        <v>3.2469666110422448</v>
+        <v>3.2469681099663132</v>
       </c>
     </row>
   </sheetData>
@@ -2283,16 +2294,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5AA7C3-FB7F-4983-AAAA-7EEF196A1E6E}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2306,7 +2319,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2320,7 +2333,7 @@
         <v>2.1702854322229599</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2334,7 +2347,7 @@
         <v>2.2160337853221361</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2348,7 +2361,7 @@
         <v>3.4697240133409442</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2362,7 +2375,7 @@
         <v>3.0346658737304941</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2376,7 +2389,7 @@
         <v>2.3832004230393857</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2390,7 +2403,7 @@
         <v>1.7826476380430927</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2404,77 +2417,77 @@
         <v>2.3909372766487413</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="6">
-        <v>14.338014061656679</v>
+        <v>14.338212462565112</v>
       </c>
       <c r="C10" s="6">
-        <v>5.6630096157766827</v>
+        <v>5.6630879771346372</v>
       </c>
       <c r="D10" s="6">
-        <v>2.2231973863499754</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
+        <v>2.2232281496327553</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="6">
-        <v>14.761505950948575</v>
+        <v>14.761596052271628</v>
       </c>
       <c r="C11" s="6">
-        <v>5.9920869299126469</v>
+        <v>5.9921235044303174</v>
       </c>
       <c r="D11" s="6">
-        <v>2.4010578192315832</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
+        <v>2.4010724748152996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="6">
-        <v>15.471745026558912</v>
+        <v>15.471801883971761</v>
       </c>
       <c r="C12" s="6">
-        <v>6.7821484521304454</v>
+        <v>6.7821733759780054</v>
       </c>
       <c r="D12" s="6">
-        <v>2.9433099917782926</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
+        <v>2.9433208082046911</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="6">
-        <v>16.906571519572243</v>
+        <v>16.906682945069651</v>
       </c>
       <c r="C13" s="6">
-        <v>7.9730577355506602</v>
+        <v>7.9731102832788032</v>
       </c>
       <c r="D13" s="6">
-        <v>3.7228012759795477</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.75">
+        <v>3.7228258117042183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="6">
-        <v>18.917807518415497</v>
+        <v>18.917874203818943</v>
       </c>
       <c r="C14" s="6">
-        <v>9.8614938648871515</v>
+        <v>9.861528626721805</v>
       </c>
       <c r="D14" s="6">
-        <v>4.96885385727236</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.75">
+        <v>4.9688713725168627</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2482,7 +2495,7 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2496,7 +2509,7 @@
         <v>3.7440315943820206</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -2510,21 +2523,21 @@
         <v>2.5122879968121774</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="6">
-        <v>14.377248283437478</v>
+        <v>14.379178100204667</v>
       </c>
       <c r="C18" s="6">
-        <v>5.9546713362898522</v>
+        <v>5.9554706147304364</v>
       </c>
       <c r="D18" s="6">
-        <v>2.3938066934341853</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.75">
+        <v>2.3941280072352225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2538,7 +2551,7 @@
         <v>2.3067387988888988</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2552,7 +2565,7 @@
         <v>2.986624568100718</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2566,7 +2579,7 @@
         <v>3.1906153094603416</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2580,32 +2593,32 @@
         <v>3.5847758943618455</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
-        <v>16.425846384233573</v>
+        <v>16.426268882370039</v>
       </c>
       <c r="C23" s="6">
-        <v>7.7074478374355584</v>
+        <v>7.7076460848970321</v>
       </c>
       <c r="D23" s="6">
-        <v>3.4256258229894185</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.75">
+        <v>3.425713935375994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="6">
-        <v>17.245560956556307</v>
+        <v>17.245555051516245</v>
       </c>
       <c r="C24" s="6">
-        <v>8.2658638827520576</v>
+        <v>8.2658610524435812</v>
       </c>
       <c r="D24" s="6">
-        <v>3.6811079784032228</v>
+        <v>3.6811067179577011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>